<commit_message>
first commit for my repository
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NaveenKhunteta/Documents/MyPOMFramework/PageObjectModel/src/main/java/com/crm/qa/testdata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{665A7912-0EF4-4390-A279-43088C37D7C6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17136" windowHeight="5412" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="deals" sheetId="2" r:id="rId2"/>
     <sheet name="tasks" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1:L15"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>title</t>
   </si>
@@ -77,12 +74,15 @@
   </si>
   <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>Flipkart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -138,6 +138,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -405,16 +408,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -442,7 +445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -456,7 +459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -468,6 +471,20 @@
       </c>
       <c r="D4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -476,24 +493,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>